<commit_message>
Update công nợ chị tuyết TPHCM.xlsx
</commit_message>
<xml_diff>
--- a/KẾ TOÁN - THÁI HẰNG/CÔNG NỢ/CHỊ TUYẾT SÀI GÒN/công nợ chị tuyết TPHCM.xlsx
+++ b/KẾ TOÁN - THÁI HẰNG/CÔNG NỢ/CHỊ TUYẾT SÀI GÒN/công nợ chị tuyết TPHCM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="hàng nhập" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="52">
   <si>
     <t>CÔNG TY CỔ PHẦN ĐT &amp; PT NANO MILK</t>
   </si>
@@ -138,9 +138,6 @@
     <t>Tổng cộng nhập hàng đợt 3</t>
   </si>
   <si>
-    <t>Tổng sau 3 đợt nhập hàng</t>
-  </si>
-  <si>
     <t xml:space="preserve">HÀNG CHỊ TUYẾT TRẢ LẠI </t>
   </si>
   <si>
@@ -150,13 +147,31 @@
     <t>Như vậy:</t>
   </si>
   <si>
-    <t>Tổng 3 lần nhập hàng (1)</t>
-  </si>
-  <si>
-    <t>Công nợ (2)-(3)</t>
-  </si>
-  <si>
     <t>Hàng trả lại  (2)</t>
+  </si>
+  <si>
+    <t>Tổng sau 4 đợt nhập hàng</t>
+  </si>
+  <si>
+    <t>Đợt 4</t>
+  </si>
+  <si>
+    <t>Tổng cộng nhập hàng đợt 4</t>
+  </si>
+  <si>
+    <t>Tổng 4 lần nhập hàng (1)</t>
+  </si>
+  <si>
+    <t>Chiết khấu 50%</t>
+  </si>
+  <si>
+    <t>Tổng doanh thu  (3) =  (1)-(2)</t>
+  </si>
+  <si>
+    <t>Đã thanh toán</t>
+  </si>
+  <si>
+    <t>Công nợ</t>
   </si>
 </sst>
 </file>
@@ -164,12 +179,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₫_-;\-* #,##0.00\ _₫_-;_-* &quot;-&quot;??\ _₫_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0\ _₫_-;\-* #,##0\ _₫_-;_-* &quot;-&quot;??\ _₫_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _₫_-;\-* #,##0.00\ _₫_-;_-* &quot;-&quot;??\ _₫_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0\ _₫_-;\-* #,##0\ _₫_-;_-* &quot;-&quot;??\ _₫_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,14 +265,21 @@
     </font>
     <font>
       <b/>
-      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -276,8 +298,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -421,13 +449,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -442,13 +494,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -461,7 +513,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
@@ -477,138 +529,128 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -651,28 +693,131 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="13" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -976,16 +1121,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P31"/>
+  <dimension ref="A1:V44"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="S43" sqref="S43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="82" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="76" customWidth="1"/>
     <col min="3" max="3" width="7" style="4" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" style="4" customWidth="1"/>
     <col min="5" max="5" width="8.85546875" style="4" customWidth="1"/>
@@ -993,16 +1138,18 @@
     <col min="7" max="7" width="7.42578125" style="4" customWidth="1"/>
     <col min="8" max="8" width="7.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.5703125" style="80" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.5703125" style="74" customWidth="1"/>
     <col min="12" max="12" width="16" style="8" customWidth="1"/>
     <col min="13" max="13" width="5.5703125" style="8" customWidth="1"/>
     <col min="14" max="14" width="5.42578125" style="8" customWidth="1"/>
     <col min="15" max="15" width="16.7109375" style="8" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="4"/>
+    <col min="16" max="21" width="9.140625" style="4"/>
+    <col min="22" max="22" width="19" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1018,7 +1165,7 @@
       <c r="M1" s="6"/>
       <c r="O1" s="6"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -1034,81 +1181,81 @@
       <c r="M2" s="13"/>
       <c r="O2" s="13"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="92" t="s">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="92"/>
-      <c r="C3" s="92"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="92"/>
-      <c r="H3" s="92"/>
-      <c r="I3" s="92"/>
-      <c r="J3" s="92"/>
-      <c r="K3" s="92"/>
-      <c r="L3" s="92"/>
-      <c r="M3" s="92"/>
-      <c r="N3" s="92"/>
-      <c r="O3" s="92"/>
-      <c r="P3" s="92"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="93"/>
-      <c r="B4" s="93"/>
-      <c r="C4" s="93"/>
-      <c r="D4" s="93"/>
-      <c r="E4" s="93"/>
-      <c r="F4" s="93"/>
-      <c r="G4" s="93"/>
-      <c r="H4" s="93"/>
-      <c r="I4" s="93"/>
-      <c r="J4" s="94"/>
-      <c r="K4" s="93"/>
-      <c r="L4" s="93"/>
-      <c r="M4" s="93"/>
-      <c r="N4" s="93"/>
-      <c r="O4" s="93"/>
-    </row>
-    <row r="5" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="95" t="s">
+      <c r="B3" s="86"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="86"/>
+      <c r="L3" s="86"/>
+      <c r="M3" s="86"/>
+      <c r="N3" s="86"/>
+      <c r="O3" s="86"/>
+      <c r="P3" s="86"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="87"/>
+      <c r="B4" s="87"/>
+      <c r="C4" s="87"/>
+      <c r="D4" s="87"/>
+      <c r="E4" s="87"/>
+      <c r="F4" s="87"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="88"/>
+      <c r="K4" s="87"/>
+      <c r="L4" s="87"/>
+      <c r="M4" s="87"/>
+      <c r="N4" s="87"/>
+      <c r="O4" s="87"/>
+    </row>
+    <row r="5" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="96" t="s">
+      <c r="B5" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="95" t="s">
+      <c r="C5" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="95" t="s">
+      <c r="D5" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="95"/>
-      <c r="F5" s="95"/>
-      <c r="G5" s="97" t="s">
+      <c r="E5" s="89"/>
+      <c r="F5" s="89"/>
+      <c r="G5" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="97"/>
-      <c r="I5" s="97"/>
-      <c r="J5" s="97"/>
-      <c r="K5" s="98"/>
-      <c r="L5" s="99" t="s">
+      <c r="H5" s="91"/>
+      <c r="I5" s="91"/>
+      <c r="J5" s="91"/>
+      <c r="K5" s="92"/>
+      <c r="L5" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="M5" s="100" t="s">
+      <c r="M5" s="94" t="s">
         <v>9</v>
       </c>
-      <c r="N5" s="100"/>
-      <c r="O5" s="100"/>
-      <c r="P5" s="101" t="s">
+      <c r="N5" s="94"/>
+      <c r="O5" s="94"/>
+      <c r="P5" s="95" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="15" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="95"/>
-      <c r="B6" s="96"/>
-      <c r="C6" s="95"/>
+    <row r="6" spans="1:22" s="15" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="89"/>
+      <c r="B6" s="90"/>
+      <c r="C6" s="89"/>
       <c r="D6" s="16" t="s">
         <v>11</v>
       </c>
@@ -1133,7 +1280,7 @@
       <c r="K6" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="L6" s="99"/>
+      <c r="L6" s="93"/>
       <c r="M6" s="19" t="s">
         <v>19</v>
       </c>
@@ -1143,252 +1290,252 @@
       <c r="O6" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="P6" s="101"/>
-    </row>
-    <row r="7" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="P6" s="95"/>
+    </row>
+    <row r="7" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="102" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="23">
+      <c r="B7" s="106">
         <v>43881</v>
       </c>
-      <c r="C7" s="24"/>
+      <c r="C7" s="109"/>
       <c r="D7" s="22" t="s">
         <v>23</v>
       </c>
       <c r="E7" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="24"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="25">
+      <c r="H7" s="24">
         <f>12*(8+4)</f>
         <v>144</v>
       </c>
-      <c r="I7" s="26">
+      <c r="I7" s="25">
         <v>485000</v>
       </c>
-      <c r="J7" s="27">
+      <c r="J7" s="26">
         <f>H7*I7</f>
         <v>69840000</v>
       </c>
-      <c r="K7" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="L7" s="27">
+      <c r="K7" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="L7" s="26">
         <f>J7*(1-K7)</f>
         <v>34920000</v>
       </c>
-      <c r="M7" s="29"/>
-      <c r="N7" s="29"/>
-      <c r="O7" s="30">
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="29">
         <f t="shared" ref="O7:O21" si="0">L7</f>
         <v>34920000</v>
       </c>
-      <c r="P7" s="25"/>
-    </row>
-    <row r="8" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="24"/>
+      <c r="P7" s="24"/>
+    </row>
+    <row r="8" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="103"/>
+      <c r="B8" s="107"/>
+      <c r="C8" s="110"/>
       <c r="D8" s="22" t="s">
         <v>23</v>
       </c>
       <c r="E8" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="24"/>
-      <c r="G8" s="32" t="s">
+      <c r="F8" s="23"/>
+      <c r="G8" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="25">
+      <c r="H8" s="24">
         <f>12*12</f>
         <v>144</v>
       </c>
-      <c r="I8" s="33">
+      <c r="I8" s="31">
         <v>465000</v>
       </c>
-      <c r="J8" s="27">
+      <c r="J8" s="26">
         <f>H8*I8</f>
         <v>66960000</v>
       </c>
-      <c r="K8" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="L8" s="27">
+      <c r="K8" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="L8" s="26">
         <f>J8*(1-K8)</f>
         <v>33480000</v>
       </c>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="30">
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="29">
         <f t="shared" si="0"/>
         <v>33480000</v>
       </c>
-      <c r="P8" s="25"/>
-    </row>
-    <row r="9" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="24"/>
+      <c r="P8" s="24"/>
+    </row>
+    <row r="9" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="103"/>
+      <c r="B9" s="107"/>
+      <c r="C9" s="110"/>
       <c r="D9" s="22" t="s">
         <v>23</v>
       </c>
       <c r="E9" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="24"/>
-      <c r="G9" s="32" t="s">
+      <c r="F9" s="23"/>
+      <c r="G9" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="25">
+      <c r="H9" s="24">
         <f>12*12</f>
         <v>144</v>
       </c>
-      <c r="I9" s="33">
+      <c r="I9" s="31">
         <v>475000</v>
       </c>
-      <c r="J9" s="27">
+      <c r="J9" s="26">
         <f>H9*I9</f>
         <v>68400000</v>
       </c>
-      <c r="K9" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="L9" s="27">
+      <c r="K9" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="L9" s="26">
         <f>J9*(1-K9)</f>
         <v>34200000</v>
       </c>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="30">
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="29">
         <f t="shared" si="0"/>
         <v>34200000</v>
       </c>
-      <c r="P9" s="25"/>
-    </row>
-    <row r="10" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="24"/>
+      <c r="P9" s="24"/>
+    </row>
+    <row r="10" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="103"/>
+      <c r="B10" s="107"/>
+      <c r="C10" s="110"/>
       <c r="D10" s="22" t="s">
         <v>23</v>
       </c>
       <c r="E10" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="24"/>
-      <c r="G10" s="32" t="s">
+      <c r="F10" s="23"/>
+      <c r="G10" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="H10" s="25">
+      <c r="H10" s="24">
         <f>12*12</f>
         <v>144</v>
       </c>
-      <c r="I10" s="33">
+      <c r="I10" s="31">
         <v>455000</v>
       </c>
-      <c r="J10" s="27">
+      <c r="J10" s="26">
         <f>H10*I10</f>
         <v>65520000</v>
       </c>
-      <c r="K10" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="L10" s="27">
+      <c r="K10" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="L10" s="26">
         <f>J10*(1-K10)</f>
         <v>32760000</v>
       </c>
-      <c r="M10" s="29"/>
-      <c r="N10" s="29"/>
-      <c r="O10" s="30">
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="29">
         <f t="shared" si="0"/>
         <v>32760000</v>
       </c>
-      <c r="P10" s="25"/>
-    </row>
-    <row r="11" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="24"/>
+      <c r="P10" s="24"/>
+    </row>
+    <row r="11" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="104"/>
+      <c r="B11" s="108"/>
+      <c r="C11" s="111"/>
       <c r="D11" s="22" t="s">
         <v>23</v>
       </c>
       <c r="E11" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="24"/>
-      <c r="G11" s="34" t="s">
+      <c r="F11" s="23"/>
+      <c r="G11" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="H11" s="25">
+      <c r="H11" s="24">
         <f>12*12</f>
         <v>144</v>
       </c>
-      <c r="I11" s="35">
+      <c r="I11" s="33">
         <v>455000</v>
       </c>
-      <c r="J11" s="27">
+      <c r="J11" s="26">
         <f>H11*I11</f>
         <v>65520000</v>
       </c>
-      <c r="K11" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="L11" s="27">
+      <c r="K11" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="L11" s="26">
         <f>J11*(1-K11)</f>
         <v>32760000</v>
       </c>
-      <c r="M11" s="29"/>
-      <c r="N11" s="29"/>
-      <c r="O11" s="30">
+      <c r="M11" s="28"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="29">
         <f t="shared" si="0"/>
         <v>32760000</v>
       </c>
-      <c r="P11" s="25"/>
-    </row>
-    <row r="12" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="85" t="s">
+      <c r="P11" s="24"/>
+    </row>
+    <row r="12" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="86"/>
-      <c r="C12" s="86"/>
-      <c r="D12" s="86"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="86"/>
-      <c r="G12" s="87"/>
-      <c r="H12" s="36">
+      <c r="B12" s="80"/>
+      <c r="C12" s="80"/>
+      <c r="D12" s="80"/>
+      <c r="E12" s="80"/>
+      <c r="F12" s="80"/>
+      <c r="G12" s="81"/>
+      <c r="H12" s="34">
         <f>SUM(H7:H11)</f>
         <v>720</v>
       </c>
-      <c r="I12" s="29"/>
-      <c r="J12" s="37">
+      <c r="I12" s="28"/>
+      <c r="J12" s="35">
         <f>SUM(J7:J11)</f>
         <v>336240000</v>
       </c>
-      <c r="K12" s="38"/>
-      <c r="L12" s="37">
+      <c r="K12" s="36"/>
+      <c r="L12" s="35">
         <f>SUM(L7:L11)</f>
         <v>168120000</v>
       </c>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29">
+      <c r="M12" s="28"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28">
         <f t="shared" si="0"/>
         <v>168120000</v>
       </c>
-      <c r="P12" s="25"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
+      <c r="P12" s="24"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" s="102" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="23">
+      <c r="B13" s="106">
         <v>43915</v>
       </c>
-      <c r="C13" s="22"/>
+      <c r="C13" s="99"/>
       <c r="D13" s="22" t="s">
         <v>23</v>
       </c>
@@ -1402,382 +1549,382 @@
       <c r="H13" s="22">
         <v>24</v>
       </c>
-      <c r="I13" s="26">
+      <c r="I13" s="25">
         <v>265000</v>
       </c>
-      <c r="J13" s="26">
+      <c r="J13" s="25">
         <f t="shared" ref="J13:J21" si="1">H13*I13</f>
         <v>6360000</v>
       </c>
-      <c r="K13" s="39">
-        <v>0.5</v>
-      </c>
-      <c r="L13" s="26">
+      <c r="K13" s="37">
+        <v>0.5</v>
+      </c>
+      <c r="L13" s="25">
         <f t="shared" ref="L13:L21" si="2">J13*(1-K13)</f>
         <v>3180000</v>
       </c>
-      <c r="M13" s="26"/>
-      <c r="N13" s="26"/>
-      <c r="O13" s="26">
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
+      <c r="O13" s="25">
         <f t="shared" si="0"/>
         <v>3180000</v>
       </c>
       <c r="P13" s="22"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
-      <c r="B14" s="40"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32" t="s">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="103"/>
+      <c r="B14" s="107"/>
+      <c r="C14" s="100"/>
+      <c r="D14" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="32" t="s">
+      <c r="E14" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32" t="s">
+      <c r="F14" s="30"/>
+      <c r="G14" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H14" s="32">
+      <c r="H14" s="30">
         <v>12</v>
       </c>
-      <c r="I14" s="33">
+      <c r="I14" s="31">
         <v>465000</v>
       </c>
-      <c r="J14" s="33">
+      <c r="J14" s="31">
         <f t="shared" si="1"/>
         <v>5580000</v>
       </c>
-      <c r="K14" s="41">
-        <v>0.5</v>
-      </c>
-      <c r="L14" s="42">
+      <c r="K14" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="L14" s="39">
         <f t="shared" si="2"/>
         <v>2790000</v>
       </c>
-      <c r="M14" s="33"/>
-      <c r="N14" s="33"/>
-      <c r="O14" s="33">
+      <c r="M14" s="31"/>
+      <c r="N14" s="31"/>
+      <c r="O14" s="31">
         <f t="shared" si="0"/>
         <v>2790000</v>
       </c>
-      <c r="P14" s="32"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
-      <c r="B15" s="40"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32" t="s">
+      <c r="P14" s="30"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="103"/>
+      <c r="B15" s="107"/>
+      <c r="C15" s="100"/>
+      <c r="D15" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="32" t="s">
+      <c r="E15" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32" t="s">
+      <c r="F15" s="30"/>
+      <c r="G15" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="H15" s="32">
+      <c r="H15" s="30">
         <v>36</v>
       </c>
-      <c r="I15" s="33">
+      <c r="I15" s="31">
         <v>475000</v>
       </c>
-      <c r="J15" s="33">
+      <c r="J15" s="31">
         <f t="shared" si="1"/>
         <v>17100000</v>
       </c>
-      <c r="K15" s="43">
-        <v>0.5</v>
-      </c>
-      <c r="L15" s="33">
+      <c r="K15" s="40">
+        <v>0.5</v>
+      </c>
+      <c r="L15" s="31">
         <f t="shared" si="2"/>
         <v>8550000</v>
       </c>
-      <c r="M15" s="33"/>
-      <c r="N15" s="33"/>
-      <c r="O15" s="33">
+      <c r="M15" s="31"/>
+      <c r="N15" s="31"/>
+      <c r="O15" s="31">
         <f t="shared" si="0"/>
         <v>8550000</v>
       </c>
-      <c r="P15" s="32"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
-      <c r="B16" s="40"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32" t="s">
+      <c r="P15" s="30"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" s="103"/>
+      <c r="B16" s="107"/>
+      <c r="C16" s="100"/>
+      <c r="D16" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="32" t="s">
+      <c r="E16" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32" t="s">
+      <c r="F16" s="30"/>
+      <c r="G16" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="H16" s="32">
+      <c r="H16" s="30">
         <v>34</v>
       </c>
-      <c r="I16" s="33">
+      <c r="I16" s="31">
         <v>485000</v>
       </c>
-      <c r="J16" s="33">
+      <c r="J16" s="31">
         <f t="shared" si="1"/>
         <v>16490000</v>
       </c>
-      <c r="K16" s="43">
-        <v>0.5</v>
-      </c>
-      <c r="L16" s="33">
+      <c r="K16" s="40">
+        <v>0.5</v>
+      </c>
+      <c r="L16" s="31">
         <f t="shared" si="2"/>
         <v>8245000</v>
       </c>
-      <c r="M16" s="33"/>
-      <c r="N16" s="33"/>
-      <c r="O16" s="33">
+      <c r="M16" s="31"/>
+      <c r="N16" s="31"/>
+      <c r="O16" s="31">
         <f t="shared" si="0"/>
         <v>8245000</v>
       </c>
-      <c r="P16" s="32"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
-      <c r="B17" s="40"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32" t="s">
+      <c r="P16" s="30"/>
+      <c r="V16" s="78"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" s="103"/>
+      <c r="B17" s="107"/>
+      <c r="C17" s="100"/>
+      <c r="D17" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="32" t="s">
+      <c r="E17" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32" t="s">
+      <c r="F17" s="30"/>
+      <c r="G17" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="H17" s="32">
+      <c r="H17" s="30">
         <v>24</v>
       </c>
-      <c r="I17" s="33">
+      <c r="I17" s="31">
         <v>485000</v>
       </c>
-      <c r="J17" s="33">
+      <c r="J17" s="31">
         <f t="shared" si="1"/>
         <v>11640000</v>
       </c>
-      <c r="K17" s="43">
-        <v>0.5</v>
-      </c>
-      <c r="L17" s="33">
+      <c r="K17" s="40">
+        <v>0.5</v>
+      </c>
+      <c r="L17" s="31">
         <f t="shared" si="2"/>
         <v>5820000</v>
       </c>
-      <c r="M17" s="33"/>
-      <c r="N17" s="33"/>
-      <c r="O17" s="33">
+      <c r="M17" s="31"/>
+      <c r="N17" s="31"/>
+      <c r="O17" s="31">
         <f t="shared" si="0"/>
         <v>5820000</v>
       </c>
-      <c r="P17" s="32"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
-      <c r="B18" s="40"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32" t="s">
+      <c r="P17" s="30"/>
+      <c r="V17" s="8"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" s="103"/>
+      <c r="B18" s="107"/>
+      <c r="C18" s="100"/>
+      <c r="D18" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="32" t="s">
+      <c r="E18" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32" t="s">
+      <c r="F18" s="30"/>
+      <c r="G18" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="H18" s="32">
+      <c r="H18" s="30">
         <v>72</v>
       </c>
-      <c r="I18" s="33">
+      <c r="I18" s="31">
         <v>550000</v>
       </c>
-      <c r="J18" s="33">
+      <c r="J18" s="31">
         <f t="shared" si="1"/>
         <v>39600000</v>
       </c>
-      <c r="K18" s="43">
-        <v>0.5</v>
-      </c>
-      <c r="L18" s="33">
+      <c r="K18" s="40">
+        <v>0.5</v>
+      </c>
+      <c r="L18" s="31">
         <f t="shared" si="2"/>
         <v>19800000</v>
       </c>
-      <c r="M18" s="33"/>
-      <c r="N18" s="33"/>
-      <c r="O18" s="33">
+      <c r="M18" s="31"/>
+      <c r="N18" s="31"/>
+      <c r="O18" s="31">
         <f t="shared" si="0"/>
         <v>19800000</v>
       </c>
-      <c r="P18" s="32"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="32"/>
-      <c r="B19" s="40"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32" t="s">
+      <c r="P18" s="30"/>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" s="103"/>
+      <c r="B19" s="107"/>
+      <c r="C19" s="100"/>
+      <c r="D19" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="32" t="s">
+      <c r="E19" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32" t="s">
+      <c r="F19" s="30"/>
+      <c r="G19" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="H19" s="32">
+      <c r="H19" s="30">
         <v>56</v>
       </c>
-      <c r="I19" s="33">
+      <c r="I19" s="31">
         <v>450000</v>
       </c>
-      <c r="J19" s="33">
+      <c r="J19" s="31">
         <f t="shared" si="1"/>
         <v>25200000</v>
       </c>
-      <c r="K19" s="43">
-        <v>0.5</v>
-      </c>
-      <c r="L19" s="33">
+      <c r="K19" s="40">
+        <v>0.5</v>
+      </c>
+      <c r="L19" s="31">
         <f t="shared" si="2"/>
         <v>12600000</v>
       </c>
-      <c r="M19" s="33"/>
-      <c r="N19" s="33"/>
-      <c r="O19" s="33">
+      <c r="M19" s="31"/>
+      <c r="N19" s="31"/>
+      <c r="O19" s="31">
         <f t="shared" si="0"/>
         <v>12600000</v>
       </c>
-      <c r="P19" s="32"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="32"/>
-      <c r="B20" s="40"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32" t="s">
+      <c r="P19" s="30"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A20" s="103"/>
+      <c r="B20" s="107"/>
+      <c r="C20" s="100"/>
+      <c r="D20" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="32" t="s">
+      <c r="E20" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32" t="s">
+      <c r="F20" s="30"/>
+      <c r="G20" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="H20" s="32">
+      <c r="H20" s="30">
         <v>36</v>
       </c>
-      <c r="I20" s="33">
+      <c r="I20" s="31">
         <v>455000</v>
       </c>
-      <c r="J20" s="33">
+      <c r="J20" s="31">
         <f t="shared" si="1"/>
         <v>16380000</v>
       </c>
-      <c r="K20" s="43">
-        <v>0.5</v>
-      </c>
-      <c r="L20" s="33">
+      <c r="K20" s="40">
+        <v>0.5</v>
+      </c>
+      <c r="L20" s="31">
         <f t="shared" si="2"/>
         <v>8190000</v>
       </c>
-      <c r="M20" s="33"/>
-      <c r="N20" s="33"/>
-      <c r="O20" s="33">
+      <c r="M20" s="31"/>
+      <c r="N20" s="31"/>
+      <c r="O20" s="31">
         <f t="shared" si="0"/>
         <v>8190000</v>
       </c>
-      <c r="P20" s="32"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="44"/>
-      <c r="B21" s="45"/>
-      <c r="C21" s="44"/>
-      <c r="D21" s="44" t="s">
+      <c r="P20" s="30"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21" s="104"/>
+      <c r="B21" s="108"/>
+      <c r="C21" s="101"/>
+      <c r="D21" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="44" t="s">
+      <c r="E21" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="44"/>
-      <c r="G21" s="44" t="s">
+      <c r="F21" s="41"/>
+      <c r="G21" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="H21" s="44">
+      <c r="H21" s="41">
         <v>12</v>
       </c>
-      <c r="I21" s="46">
+      <c r="I21" s="42">
         <v>455000</v>
       </c>
-      <c r="J21" s="46">
+      <c r="J21" s="42">
         <f t="shared" si="1"/>
         <v>5460000</v>
       </c>
-      <c r="K21" s="47">
-        <v>0.5</v>
-      </c>
-      <c r="L21" s="46">
+      <c r="K21" s="43">
+        <v>0.5</v>
+      </c>
+      <c r="L21" s="42">
         <f t="shared" si="2"/>
         <v>2730000</v>
       </c>
-      <c r="M21" s="46"/>
-      <c r="N21" s="46"/>
-      <c r="O21" s="46">
+      <c r="M21" s="42"/>
+      <c r="N21" s="42"/>
+      <c r="O21" s="42">
         <f t="shared" si="0"/>
         <v>2730000</v>
       </c>
-      <c r="P21" s="44"/>
-    </row>
-    <row r="22" spans="1:16" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="85" t="s">
+      <c r="P21" s="41"/>
+    </row>
+    <row r="22" spans="1:22" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="79" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="86"/>
-      <c r="C22" s="86"/>
-      <c r="D22" s="86"/>
-      <c r="E22" s="86"/>
-      <c r="F22" s="86"/>
-      <c r="G22" s="87"/>
-      <c r="H22" s="48">
+      <c r="B22" s="80"/>
+      <c r="C22" s="80"/>
+      <c r="D22" s="80"/>
+      <c r="E22" s="80"/>
+      <c r="F22" s="80"/>
+      <c r="G22" s="81"/>
+      <c r="H22" s="44">
         <f>SUM(H13:H21)</f>
         <v>306</v>
       </c>
-      <c r="I22" s="49"/>
-      <c r="J22" s="49">
+      <c r="I22" s="45"/>
+      <c r="J22" s="45">
         <f>SUM(J13:J21)</f>
         <v>143810000</v>
       </c>
-      <c r="K22" s="50">
-        <v>0.5</v>
-      </c>
-      <c r="L22" s="49">
+      <c r="K22" s="46"/>
+      <c r="L22" s="45">
         <f>SUM(L13:L21)</f>
         <v>71905000</v>
       </c>
-      <c r="M22" s="49"/>
-      <c r="N22" s="49"/>
-      <c r="O22" s="49">
+      <c r="M22" s="45"/>
+      <c r="N22" s="45"/>
+      <c r="O22" s="45">
         <f>SUM(O13:O21)</f>
         <v>71905000</v>
       </c>
-      <c r="P22" s="48"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="22" t="s">
+      <c r="P22" s="44"/>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="23">
+      <c r="B23" s="115">
         <v>43916</v>
       </c>
-      <c r="C23" s="22"/>
+      <c r="C23" s="102"/>
       <c r="D23" s="22" t="s">
         <v>23</v>
       </c>
@@ -1791,334 +1938,694 @@
       <c r="H23" s="22">
         <v>36</v>
       </c>
-      <c r="I23" s="26">
+      <c r="I23" s="25">
         <v>455000</v>
       </c>
-      <c r="J23" s="26">
+      <c r="J23" s="25">
         <f t="shared" ref="J23:J29" si="3">I23*H23</f>
         <v>16380000</v>
       </c>
-      <c r="K23" s="41">
-        <v>0.5</v>
-      </c>
-      <c r="L23" s="42">
+      <c r="K23" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="L23" s="39">
         <f t="shared" ref="L23:L29" si="4">J23*(1-K23)</f>
         <v>8190000</v>
       </c>
-      <c r="M23" s="26"/>
-      <c r="N23" s="26"/>
-      <c r="O23" s="26">
+      <c r="M23" s="25"/>
+      <c r="N23" s="25"/>
+      <c r="O23" s="25">
         <f t="shared" ref="O23:O29" si="5">L23</f>
         <v>8190000</v>
       </c>
       <c r="P23" s="22"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32" t="s">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24" s="113"/>
+      <c r="B24" s="116"/>
+      <c r="C24" s="103"/>
+      <c r="D24" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="E24" s="32" t="s">
+      <c r="E24" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="32"/>
-      <c r="G24" s="32" t="s">
+      <c r="F24" s="30"/>
+      <c r="G24" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="H24" s="32">
+      <c r="H24" s="30">
         <v>36</v>
       </c>
-      <c r="I24" s="33">
+      <c r="I24" s="31">
         <v>475000</v>
       </c>
-      <c r="J24" s="33">
+      <c r="J24" s="31">
         <f t="shared" si="3"/>
         <v>17100000</v>
       </c>
-      <c r="K24" s="43">
-        <v>0.5</v>
-      </c>
-      <c r="L24" s="33">
+      <c r="K24" s="40">
+        <v>0.5</v>
+      </c>
+      <c r="L24" s="31">
         <f t="shared" si="4"/>
         <v>8550000</v>
       </c>
-      <c r="M24" s="33"/>
-      <c r="N24" s="33"/>
-      <c r="O24" s="33">
+      <c r="M24" s="31"/>
+      <c r="N24" s="31"/>
+      <c r="O24" s="31">
         <f t="shared" si="5"/>
         <v>8550000</v>
       </c>
-      <c r="P24" s="32"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="32"/>
-      <c r="B25" s="40"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32" t="s">
+      <c r="P24" s="30"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25" s="113"/>
+      <c r="B25" s="116"/>
+      <c r="C25" s="103"/>
+      <c r="D25" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="E25" s="32" t="s">
+      <c r="E25" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="F25" s="32"/>
-      <c r="G25" s="32" t="s">
+      <c r="F25" s="30"/>
+      <c r="G25" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="H25" s="32">
+      <c r="H25" s="30">
         <v>36</v>
       </c>
-      <c r="I25" s="33">
+      <c r="I25" s="31">
         <v>485000</v>
       </c>
-      <c r="J25" s="33">
+      <c r="J25" s="31">
         <f t="shared" si="3"/>
         <v>17460000</v>
       </c>
-      <c r="K25" s="43">
-        <v>0.5</v>
-      </c>
-      <c r="L25" s="33">
+      <c r="K25" s="40">
+        <v>0.5</v>
+      </c>
+      <c r="L25" s="31">
         <f t="shared" si="4"/>
         <v>8730000</v>
       </c>
-      <c r="M25" s="33"/>
-      <c r="N25" s="33"/>
-      <c r="O25" s="33">
+      <c r="M25" s="31"/>
+      <c r="N25" s="31"/>
+      <c r="O25" s="31">
         <f t="shared" si="5"/>
         <v>8730000</v>
       </c>
-      <c r="P25" s="32"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="32"/>
-      <c r="B26" s="40"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32" t="s">
+      <c r="P25" s="30"/>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26" s="113"/>
+      <c r="B26" s="116"/>
+      <c r="C26" s="103"/>
+      <c r="D26" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="E26" s="32" t="s">
+      <c r="E26" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="32"/>
-      <c r="G26" s="32" t="s">
+      <c r="F26" s="30"/>
+      <c r="G26" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="H26" s="32">
+      <c r="H26" s="30">
         <v>36</v>
       </c>
-      <c r="I26" s="33">
+      <c r="I26" s="31">
         <v>485000</v>
       </c>
-      <c r="J26" s="33">
+      <c r="J26" s="31">
         <f t="shared" si="3"/>
         <v>17460000</v>
       </c>
-      <c r="K26" s="43">
-        <v>0.5</v>
-      </c>
-      <c r="L26" s="33">
+      <c r="K26" s="40">
+        <v>0.5</v>
+      </c>
+      <c r="L26" s="31">
         <f t="shared" si="4"/>
         <v>8730000</v>
       </c>
-      <c r="M26" s="33"/>
-      <c r="N26" s="33"/>
-      <c r="O26" s="33">
+      <c r="M26" s="31"/>
+      <c r="N26" s="31"/>
+      <c r="O26" s="31">
         <f t="shared" si="5"/>
         <v>8730000</v>
       </c>
-      <c r="P26" s="32"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="32"/>
-      <c r="B27" s="40"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32" t="s">
+      <c r="P26" s="30"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A27" s="113"/>
+      <c r="B27" s="116"/>
+      <c r="C27" s="103"/>
+      <c r="D27" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="E27" s="32" t="s">
+      <c r="E27" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="F27" s="32"/>
-      <c r="G27" s="32" t="s">
+      <c r="F27" s="30"/>
+      <c r="G27" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="H27" s="32">
+      <c r="H27" s="30">
         <v>72</v>
       </c>
-      <c r="I27" s="33">
+      <c r="I27" s="31">
         <v>550000</v>
       </c>
-      <c r="J27" s="33">
+      <c r="J27" s="31">
         <f t="shared" si="3"/>
         <v>39600000</v>
       </c>
-      <c r="K27" s="43">
-        <v>0.5</v>
-      </c>
-      <c r="L27" s="33">
+      <c r="K27" s="40">
+        <v>0.5</v>
+      </c>
+      <c r="L27" s="31">
         <f t="shared" si="4"/>
         <v>19800000</v>
       </c>
-      <c r="M27" s="33"/>
-      <c r="N27" s="33"/>
-      <c r="O27" s="33">
+      <c r="M27" s="31"/>
+      <c r="N27" s="31"/>
+      <c r="O27" s="31">
         <f t="shared" si="5"/>
         <v>19800000</v>
       </c>
-      <c r="P27" s="32"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="32"/>
-      <c r="B28" s="40"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32" t="s">
+      <c r="P27" s="30"/>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A28" s="113"/>
+      <c r="B28" s="116"/>
+      <c r="C28" s="103"/>
+      <c r="D28" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="32" t="s">
+      <c r="E28" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32" t="s">
+      <c r="F28" s="30"/>
+      <c r="G28" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="H28" s="32">
+      <c r="H28" s="30">
         <v>36</v>
       </c>
-      <c r="I28" s="33">
+      <c r="I28" s="31">
         <v>455000</v>
       </c>
-      <c r="J28" s="33">
+      <c r="J28" s="31">
         <f t="shared" si="3"/>
         <v>16380000</v>
       </c>
-      <c r="K28" s="43">
-        <v>0.5</v>
-      </c>
-      <c r="L28" s="33">
+      <c r="K28" s="40">
+        <v>0.5</v>
+      </c>
+      <c r="L28" s="31">
         <f t="shared" si="4"/>
         <v>8190000</v>
       </c>
-      <c r="M28" s="33"/>
-      <c r="N28" s="33"/>
-      <c r="O28" s="33">
+      <c r="M28" s="31"/>
+      <c r="N28" s="31"/>
+      <c r="O28" s="31">
         <f t="shared" si="5"/>
         <v>8190000</v>
       </c>
-      <c r="P28" s="32"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="34"/>
-      <c r="B29" s="52"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34" t="s">
+      <c r="P28" s="30"/>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A29" s="114"/>
+      <c r="B29" s="117"/>
+      <c r="C29" s="104"/>
+      <c r="D29" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="E29" s="34" t="s">
+      <c r="E29" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="F29" s="34"/>
-      <c r="G29" s="34" t="s">
+      <c r="F29" s="32"/>
+      <c r="G29" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="H29" s="34">
+      <c r="H29" s="32">
         <v>36</v>
       </c>
-      <c r="I29" s="35">
+      <c r="I29" s="33">
         <v>455000</v>
       </c>
-      <c r="J29" s="35">
+      <c r="J29" s="33">
         <f t="shared" si="3"/>
         <v>16380000</v>
       </c>
-      <c r="K29" s="47">
-        <v>0.5</v>
-      </c>
-      <c r="L29" s="46">
+      <c r="K29" s="43">
+        <v>0.5</v>
+      </c>
+      <c r="L29" s="42">
         <f t="shared" si="4"/>
         <v>8190000</v>
       </c>
-      <c r="M29" s="35"/>
-      <c r="N29" s="35"/>
-      <c r="O29" s="35">
+      <c r="M29" s="33"/>
+      <c r="N29" s="33"/>
+      <c r="O29" s="33">
         <f t="shared" si="5"/>
         <v>8190000</v>
       </c>
-      <c r="P29" s="34"/>
-    </row>
-    <row r="30" spans="1:16" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="88" t="s">
+      <c r="P29" s="32"/>
+    </row>
+    <row r="30" spans="1:22" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="88"/>
-      <c r="C30" s="88"/>
-      <c r="D30" s="88"/>
-      <c r="E30" s="88"/>
-      <c r="F30" s="88"/>
-      <c r="G30" s="88"/>
-      <c r="H30" s="48">
+      <c r="B30" s="82"/>
+      <c r="C30" s="82"/>
+      <c r="D30" s="82"/>
+      <c r="E30" s="82"/>
+      <c r="F30" s="82"/>
+      <c r="G30" s="82"/>
+      <c r="H30" s="44">
         <f>SUM(H23:H29)</f>
         <v>288</v>
       </c>
-      <c r="I30" s="49"/>
-      <c r="J30" s="49">
+      <c r="I30" s="45"/>
+      <c r="J30" s="45">
         <f>SUM(J23:J29)</f>
         <v>140760000</v>
       </c>
-      <c r="K30" s="50">
-        <v>0.5</v>
-      </c>
-      <c r="L30" s="49">
+      <c r="K30" s="46"/>
+      <c r="L30" s="45">
         <f>SUM(L23:L29)</f>
         <v>70380000</v>
       </c>
-      <c r="M30" s="49"/>
-      <c r="N30" s="49"/>
-      <c r="O30" s="49">
+      <c r="M30" s="45"/>
+      <c r="N30" s="45"/>
+      <c r="O30" s="45">
         <f>SUM(O23:O29)</f>
         <v>70380000</v>
       </c>
-      <c r="P30" s="48"/>
-    </row>
-    <row r="31" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="89" t="s">
-        <v>40</v>
-      </c>
-      <c r="B31" s="90"/>
-      <c r="C31" s="90"/>
-      <c r="D31" s="90"/>
-      <c r="E31" s="90"/>
-      <c r="F31" s="90"/>
-      <c r="G31" s="91"/>
-      <c r="H31" s="53">
-        <f>H30+H22+H12</f>
-        <v>1314</v>
-      </c>
-      <c r="I31" s="54"/>
-      <c r="J31" s="54">
-        <f>J30+J22+J12</f>
-        <v>620810000</v>
-      </c>
-      <c r="K31" s="55"/>
-      <c r="L31" s="54">
-        <f>L30+L22+L12</f>
-        <v>310405000</v>
-      </c>
-      <c r="M31" s="54"/>
-      <c r="N31" s="54"/>
-      <c r="O31" s="54">
-        <f>O30+O22+O12</f>
-        <v>310405000</v>
-      </c>
-      <c r="P31" s="53"/>
+      <c r="P30" s="44"/>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A31" s="102" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" s="106">
+        <v>44032</v>
+      </c>
+      <c r="C31" s="99"/>
+      <c r="D31" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="E31" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="H31" s="22">
+        <v>300</v>
+      </c>
+      <c r="I31" s="25">
+        <v>455000</v>
+      </c>
+      <c r="J31" s="25">
+        <f>H31*I31</f>
+        <v>136500000</v>
+      </c>
+      <c r="K31" s="37">
+        <v>0.5</v>
+      </c>
+      <c r="L31" s="25">
+        <f>J31*(1-K31)</f>
+        <v>68250000</v>
+      </c>
+      <c r="M31" s="25"/>
+      <c r="N31" s="25"/>
+      <c r="O31" s="25">
+        <f>L31</f>
+        <v>68250000</v>
+      </c>
+      <c r="P31" s="22"/>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A32" s="103"/>
+      <c r="B32" s="107"/>
+      <c r="C32" s="100"/>
+      <c r="D32" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="F32" s="30"/>
+      <c r="G32" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="H32" s="30">
+        <v>180</v>
+      </c>
+      <c r="I32" s="31">
+        <v>465000</v>
+      </c>
+      <c r="J32" s="31">
+        <f t="shared" ref="J32:J38" si="6">H32*I32</f>
+        <v>83700000</v>
+      </c>
+      <c r="K32" s="40">
+        <v>0.5</v>
+      </c>
+      <c r="L32" s="31">
+        <f t="shared" ref="L32:L38" si="7">J32*(1-K32)</f>
+        <v>41850000</v>
+      </c>
+      <c r="M32" s="31"/>
+      <c r="N32" s="31"/>
+      <c r="O32" s="31">
+        <f t="shared" ref="O32:O39" si="8">L32</f>
+        <v>41850000</v>
+      </c>
+      <c r="P32" s="30"/>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A33" s="103"/>
+      <c r="B33" s="107"/>
+      <c r="C33" s="100"/>
+      <c r="D33" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" s="30"/>
+      <c r="G33" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="H33" s="30">
+        <v>120</v>
+      </c>
+      <c r="I33" s="31">
+        <v>475000</v>
+      </c>
+      <c r="J33" s="31">
+        <f t="shared" si="6"/>
+        <v>57000000</v>
+      </c>
+      <c r="K33" s="40">
+        <v>0.5</v>
+      </c>
+      <c r="L33" s="31">
+        <f t="shared" si="7"/>
+        <v>28500000</v>
+      </c>
+      <c r="M33" s="31"/>
+      <c r="N33" s="31"/>
+      <c r="O33" s="31">
+        <f t="shared" si="8"/>
+        <v>28500000</v>
+      </c>
+      <c r="P33" s="30"/>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A34" s="103"/>
+      <c r="B34" s="107"/>
+      <c r="C34" s="100"/>
+      <c r="D34" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="E34" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="F34" s="30"/>
+      <c r="G34" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="H34" s="30">
+        <v>240</v>
+      </c>
+      <c r="I34" s="31">
+        <v>485000</v>
+      </c>
+      <c r="J34" s="31">
+        <f t="shared" si="6"/>
+        <v>116400000</v>
+      </c>
+      <c r="K34" s="40">
+        <v>0.5</v>
+      </c>
+      <c r="L34" s="31">
+        <f t="shared" si="7"/>
+        <v>58200000</v>
+      </c>
+      <c r="M34" s="31"/>
+      <c r="N34" s="31"/>
+      <c r="O34" s="31">
+        <f t="shared" si="8"/>
+        <v>58200000</v>
+      </c>
+      <c r="P34" s="30"/>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A35" s="103"/>
+      <c r="B35" s="107"/>
+      <c r="C35" s="100"/>
+      <c r="D35" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="E35" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="F35" s="30"/>
+      <c r="G35" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="H35" s="30">
+        <v>60</v>
+      </c>
+      <c r="I35" s="31">
+        <v>485000</v>
+      </c>
+      <c r="J35" s="31">
+        <f t="shared" si="6"/>
+        <v>29100000</v>
+      </c>
+      <c r="K35" s="40">
+        <v>0.5</v>
+      </c>
+      <c r="L35" s="31">
+        <f t="shared" si="7"/>
+        <v>14550000</v>
+      </c>
+      <c r="M35" s="31"/>
+      <c r="N35" s="31"/>
+      <c r="O35" s="31">
+        <f t="shared" si="8"/>
+        <v>14550000</v>
+      </c>
+      <c r="P35" s="30"/>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A36" s="103"/>
+      <c r="B36" s="107"/>
+      <c r="C36" s="100"/>
+      <c r="D36" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="E36" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="F36" s="30"/>
+      <c r="G36" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="H36" s="30">
+        <v>240</v>
+      </c>
+      <c r="I36" s="31">
+        <v>550000</v>
+      </c>
+      <c r="J36" s="31">
+        <f t="shared" si="6"/>
+        <v>132000000</v>
+      </c>
+      <c r="K36" s="40">
+        <v>0.5</v>
+      </c>
+      <c r="L36" s="31">
+        <f t="shared" si="7"/>
+        <v>66000000</v>
+      </c>
+      <c r="M36" s="31"/>
+      <c r="N36" s="31"/>
+      <c r="O36" s="31">
+        <f t="shared" si="8"/>
+        <v>66000000</v>
+      </c>
+      <c r="P36" s="30"/>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A37" s="103"/>
+      <c r="B37" s="107"/>
+      <c r="C37" s="100"/>
+      <c r="D37" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="E37" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="F37" s="30"/>
+      <c r="G37" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="H37" s="30">
+        <v>84</v>
+      </c>
+      <c r="I37" s="31">
+        <v>455000</v>
+      </c>
+      <c r="J37" s="31">
+        <f t="shared" si="6"/>
+        <v>38220000</v>
+      </c>
+      <c r="K37" s="40">
+        <v>0.5</v>
+      </c>
+      <c r="L37" s="31">
+        <f t="shared" si="7"/>
+        <v>19110000</v>
+      </c>
+      <c r="M37" s="31"/>
+      <c r="N37" s="31"/>
+      <c r="O37" s="31">
+        <f t="shared" si="8"/>
+        <v>19110000</v>
+      </c>
+      <c r="P37" s="30"/>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A38" s="104"/>
+      <c r="B38" s="108"/>
+      <c r="C38" s="101"/>
+      <c r="D38" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="E38" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="F38" s="32"/>
+      <c r="G38" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="H38" s="32">
+        <v>240</v>
+      </c>
+      <c r="I38" s="33">
+        <v>455000</v>
+      </c>
+      <c r="J38" s="33">
+        <f t="shared" si="6"/>
+        <v>109200000</v>
+      </c>
+      <c r="K38" s="118">
+        <v>0.5</v>
+      </c>
+      <c r="L38" s="33">
+        <f t="shared" si="7"/>
+        <v>54600000</v>
+      </c>
+      <c r="M38" s="33"/>
+      <c r="N38" s="33"/>
+      <c r="O38" s="33">
+        <f t="shared" si="8"/>
+        <v>54600000</v>
+      </c>
+      <c r="P38" s="32"/>
+    </row>
+    <row r="39" spans="1:22" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="82" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" s="82"/>
+      <c r="C39" s="82"/>
+      <c r="D39" s="82"/>
+      <c r="E39" s="82"/>
+      <c r="F39" s="82"/>
+      <c r="G39" s="82"/>
+      <c r="H39" s="44">
+        <f>SUM(H31:H38)</f>
+        <v>1464</v>
+      </c>
+      <c r="I39" s="45"/>
+      <c r="J39" s="45">
+        <f>SUM(J31:J38)</f>
+        <v>702120000</v>
+      </c>
+      <c r="K39" s="46"/>
+      <c r="L39" s="45">
+        <f>SUM(L31:L38)</f>
+        <v>351060000</v>
+      </c>
+      <c r="M39" s="45"/>
+      <c r="N39" s="45"/>
+      <c r="O39" s="45">
+        <f t="shared" si="8"/>
+        <v>351060000</v>
+      </c>
+      <c r="P39" s="44"/>
+    </row>
+    <row r="40" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="83" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40" s="84"/>
+      <c r="C40" s="84"/>
+      <c r="D40" s="84"/>
+      <c r="E40" s="84"/>
+      <c r="F40" s="84"/>
+      <c r="G40" s="85"/>
+      <c r="H40" s="48">
+        <f>H30+H22+H12+H39</f>
+        <v>2778</v>
+      </c>
+      <c r="I40" s="49"/>
+      <c r="J40" s="49">
+        <f>J30+J22+J12+J39</f>
+        <v>1322930000</v>
+      </c>
+      <c r="K40" s="49"/>
+      <c r="L40" s="49">
+        <f>L30+L22+L12+L39</f>
+        <v>661465000</v>
+      </c>
+      <c r="M40" s="49"/>
+      <c r="N40" s="49"/>
+      <c r="O40" s="49">
+        <f>O30+O22+O12+O39</f>
+        <v>661465000</v>
+      </c>
+      <c r="P40" s="48"/>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V44" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="27">
+    <mergeCell ref="A39:G39"/>
+    <mergeCell ref="A31:A38"/>
+    <mergeCell ref="B31:B38"/>
+    <mergeCell ref="C31:C38"/>
+    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="B13:B21"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="C13:C21"/>
+    <mergeCell ref="A23:A29"/>
+    <mergeCell ref="B23:B29"/>
+    <mergeCell ref="C23:C29"/>
     <mergeCell ref="A12:G12"/>
     <mergeCell ref="A22:G22"/>
     <mergeCell ref="A30:G30"/>
-    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="A40:G40"/>
     <mergeCell ref="A3:P3"/>
     <mergeCell ref="A4:O4"/>
     <mergeCell ref="A5:A6"/>
@@ -2129,116 +2636,125 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:O5"/>
     <mergeCell ref="P5:P6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="B7:B11"/>
   </mergeCells>
   <pageMargins left="0.17" right="0.2" top="0.45" bottom="0.32" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S18"/>
+  <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.85546875" customWidth="1"/>
     <col min="2" max="2" width="11.140625" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.42578125" customWidth="1"/>
     <col min="11" max="11" width="6" customWidth="1"/>
     <col min="12" max="12" width="14.42578125" customWidth="1"/>
     <col min="13" max="13" width="5.28515625" customWidth="1"/>
     <col min="14" max="14" width="5" customWidth="1"/>
     <col min="15" max="15" width="14.5703125" customWidth="1"/>
-    <col min="19" max="19" width="16" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.140625" style="132" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="58" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:21" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="I1" s="59"/>
-    </row>
-    <row r="2" spans="1:19" s="58" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="60" t="s">
+      <c r="B1" s="51"/>
+      <c r="I1" s="53"/>
+      <c r="S1" s="129"/>
+    </row>
+    <row r="2" spans="1:21" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="I2" s="59"/>
-    </row>
-    <row r="3" spans="1:19" s="58" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="102" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="102"/>
-      <c r="C3" s="102"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="102"/>
-      <c r="F3" s="102"/>
-      <c r="G3" s="102"/>
-      <c r="H3" s="102"/>
-      <c r="I3" s="102"/>
-      <c r="J3" s="102"/>
-      <c r="K3" s="102"/>
-      <c r="L3" s="102"/>
-      <c r="M3" s="102"/>
-      <c r="N3" s="102"/>
-      <c r="O3" s="102"/>
-      <c r="P3" s="102"/>
-    </row>
-    <row r="4" spans="1:19" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="82"/>
+      <c r="B2" s="51"/>
+      <c r="I2" s="53"/>
+      <c r="S2" s="129"/>
+    </row>
+    <row r="3" spans="1:21" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="97" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="97"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+      <c r="N3" s="97"/>
+      <c r="O3" s="97"/>
+      <c r="P3" s="97"/>
+      <c r="S3" s="129"/>
+    </row>
+    <row r="4" spans="1:21" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="76"/>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
-      <c r="K4" s="80"/>
+      <c r="K4" s="74"/>
       <c r="L4" s="8"/>
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
       <c r="O4" s="8"/>
-    </row>
-    <row r="5" spans="1:19" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="95" t="s">
+      <c r="S4" s="76"/>
+    </row>
+    <row r="5" spans="1:21" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="96" t="s">
+      <c r="B5" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="95" t="s">
+      <c r="C5" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="95" t="s">
+      <c r="D5" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="95"/>
-      <c r="F5" s="95"/>
-      <c r="G5" s="97" t="s">
+      <c r="E5" s="89"/>
+      <c r="F5" s="89"/>
+      <c r="G5" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="97"/>
-      <c r="I5" s="97"/>
-      <c r="J5" s="97"/>
-      <c r="K5" s="98"/>
-      <c r="L5" s="99" t="s">
+      <c r="H5" s="91"/>
+      <c r="I5" s="91"/>
+      <c r="J5" s="91"/>
+      <c r="K5" s="92"/>
+      <c r="L5" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="M5" s="100" t="s">
+      <c r="M5" s="94" t="s">
         <v>9</v>
       </c>
-      <c r="N5" s="100"/>
-      <c r="O5" s="100"/>
-      <c r="P5" s="101" t="s">
+      <c r="N5" s="94"/>
+      <c r="O5" s="94"/>
+      <c r="P5" s="95" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" s="15" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="95"/>
-      <c r="B6" s="96"/>
-      <c r="C6" s="95"/>
+      <c r="S5" s="130"/>
+    </row>
+    <row r="6" spans="1:21" s="15" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="89"/>
+      <c r="B6" s="90"/>
+      <c r="C6" s="89"/>
       <c r="D6" s="16" t="s">
         <v>11</v>
       </c>
@@ -2263,7 +2779,7 @@
       <c r="K6" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="L6" s="99"/>
+      <c r="L6" s="93"/>
       <c r="M6" s="19" t="s">
         <v>19</v>
       </c>
@@ -2273,328 +2789,473 @@
       <c r="O6" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="P6" s="101"/>
-    </row>
-    <row r="7" spans="1:19" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="23">
+      <c r="P6" s="95"/>
+      <c r="S6" s="130"/>
+      <c r="U6" s="4"/>
+    </row>
+    <row r="7" spans="1:21" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="102"/>
+      <c r="B7" s="106">
         <v>43881</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22" t="s">
+      <c r="C7" s="102"/>
+      <c r="D7" s="102" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="102" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="22"/>
+      <c r="F7" s="102"/>
       <c r="G7" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="61">
+      <c r="H7" s="55">
         <f>8*12</f>
         <v>96</v>
       </c>
-      <c r="I7" s="26">
+      <c r="I7" s="25">
         <v>485000</v>
       </c>
-      <c r="J7" s="62">
+      <c r="J7" s="56">
         <f>H7*I7</f>
         <v>46560000</v>
       </c>
-      <c r="K7" s="63">
-        <v>0.5</v>
-      </c>
-      <c r="L7" s="62">
+      <c r="K7" s="57">
+        <v>0.5</v>
+      </c>
+      <c r="L7" s="56">
         <f>J7*(1-K7)</f>
         <v>23280000</v>
       </c>
-      <c r="M7" s="64"/>
-      <c r="N7" s="64"/>
-      <c r="O7" s="65">
-        <f t="shared" ref="O7:O12" si="0">L7</f>
+      <c r="M7" s="58"/>
+      <c r="N7" s="58"/>
+      <c r="O7" s="59">
+        <f t="shared" ref="O7:O13" si="0">L7</f>
         <v>23280000</v>
       </c>
       <c r="P7" s="22"/>
-    </row>
-    <row r="8" spans="1:19" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32" t="s">
+      <c r="S7" s="76"/>
+    </row>
+    <row r="8" spans="1:21" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="103"/>
+      <c r="B8" s="107"/>
+      <c r="C8" s="103"/>
+      <c r="D8" s="103"/>
+      <c r="E8" s="103"/>
+      <c r="F8" s="103"/>
+      <c r="G8" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="66">
+      <c r="H8" s="60">
         <f>8*12</f>
         <v>96</v>
       </c>
-      <c r="I8" s="33">
+      <c r="I8" s="31">
         <v>465000</v>
       </c>
-      <c r="J8" s="67">
+      <c r="J8" s="61">
         <f>H8*I8</f>
         <v>44640000</v>
       </c>
-      <c r="K8" s="68">
-        <v>0.5</v>
-      </c>
-      <c r="L8" s="67">
+      <c r="K8" s="62">
+        <v>0.5</v>
+      </c>
+      <c r="L8" s="61">
         <f>J8*(1-K8)</f>
         <v>22320000</v>
       </c>
-      <c r="M8" s="69"/>
-      <c r="N8" s="69"/>
-      <c r="O8" s="70">
+      <c r="M8" s="63"/>
+      <c r="N8" s="63"/>
+      <c r="O8" s="64">
         <f t="shared" si="0"/>
         <v>22320000</v>
       </c>
-      <c r="P8" s="32"/>
-    </row>
-    <row r="9" spans="1:19" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
-      <c r="B9" s="40"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32" t="s">
+      <c r="P8" s="30"/>
+      <c r="S8" s="76"/>
+    </row>
+    <row r="9" spans="1:21" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="103"/>
+      <c r="B9" s="107"/>
+      <c r="C9" s="103"/>
+      <c r="D9" s="103"/>
+      <c r="E9" s="103"/>
+      <c r="F9" s="103"/>
+      <c r="G9" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="66">
+      <c r="H9" s="60">
         <f>11*12</f>
         <v>132</v>
       </c>
-      <c r="I9" s="33">
+      <c r="I9" s="31">
         <v>475000</v>
       </c>
-      <c r="J9" s="67">
+      <c r="J9" s="61">
         <f>H9*I9</f>
         <v>62700000</v>
       </c>
-      <c r="K9" s="68">
-        <v>0.5</v>
-      </c>
-      <c r="L9" s="67">
+      <c r="K9" s="62">
+        <v>0.5</v>
+      </c>
+      <c r="L9" s="61">
         <f>J9*(1-K9)</f>
         <v>31350000</v>
       </c>
-      <c r="M9" s="69"/>
-      <c r="N9" s="69"/>
-      <c r="O9" s="70">
+      <c r="M9" s="63"/>
+      <c r="N9" s="63"/>
+      <c r="O9" s="64">
         <f t="shared" si="0"/>
         <v>31350000</v>
       </c>
-      <c r="P9" s="32"/>
-    </row>
-    <row r="10" spans="1:19" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="40"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32" t="s">
+      <c r="P9" s="30"/>
+      <c r="S9" s="76"/>
+    </row>
+    <row r="10" spans="1:21" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="103"/>
+      <c r="B10" s="107"/>
+      <c r="C10" s="103"/>
+      <c r="D10" s="103"/>
+      <c r="E10" s="103"/>
+      <c r="F10" s="103"/>
+      <c r="G10" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="H10" s="66">
+      <c r="H10" s="60">
         <f>9*12</f>
         <v>108</v>
       </c>
-      <c r="I10" s="33">
+      <c r="I10" s="31">
         <v>455000</v>
       </c>
-      <c r="J10" s="67">
+      <c r="J10" s="61">
         <f>H10*I10</f>
         <v>49140000</v>
       </c>
-      <c r="K10" s="68">
-        <v>0.5</v>
-      </c>
-      <c r="L10" s="67">
+      <c r="K10" s="62">
+        <v>0.5</v>
+      </c>
+      <c r="L10" s="61">
         <f>J10*(1-K10)</f>
         <v>24570000</v>
       </c>
-      <c r="M10" s="69"/>
-      <c r="N10" s="69"/>
-      <c r="O10" s="70">
+      <c r="M10" s="63"/>
+      <c r="N10" s="63"/>
+      <c r="O10" s="64">
         <f t="shared" si="0"/>
         <v>24570000</v>
       </c>
-      <c r="P10" s="32"/>
-      <c r="S10" s="106"/>
-    </row>
-    <row r="11" spans="1:19" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="44"/>
-      <c r="B11" s="45"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44" t="s">
+      <c r="P10" s="30"/>
+      <c r="S10" s="76"/>
+    </row>
+    <row r="11" spans="1:21" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="103"/>
+      <c r="B11" s="107"/>
+      <c r="C11" s="103"/>
+      <c r="D11" s="103"/>
+      <c r="E11" s="103"/>
+      <c r="F11" s="103"/>
+      <c r="G11" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="H11" s="71">
+      <c r="H11" s="65">
         <f>7*12</f>
         <v>84</v>
       </c>
-      <c r="I11" s="46">
+      <c r="I11" s="42">
         <v>455000</v>
       </c>
-      <c r="J11" s="72">
+      <c r="J11" s="66">
         <f>H11*I11</f>
         <v>38220000</v>
       </c>
-      <c r="K11" s="73">
-        <v>0.5</v>
-      </c>
-      <c r="L11" s="72">
+      <c r="K11" s="67">
+        <v>0.5</v>
+      </c>
+      <c r="L11" s="66">
         <f>J11*(1-K11)</f>
         <v>19110000</v>
       </c>
-      <c r="M11" s="74"/>
-      <c r="N11" s="74"/>
-      <c r="O11" s="75">
+      <c r="M11" s="68"/>
+      <c r="N11" s="68"/>
+      <c r="O11" s="69">
         <f t="shared" si="0"/>
         <v>19110000</v>
       </c>
-      <c r="P11" s="44"/>
-    </row>
-    <row r="12" spans="1:19" s="51" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="88" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" s="88"/>
-      <c r="C12" s="88"/>
-      <c r="D12" s="88"/>
-      <c r="E12" s="88"/>
-      <c r="F12" s="88"/>
-      <c r="G12" s="88"/>
-      <c r="H12" s="48">
-        <f>SUM(H7:H11)</f>
-        <v>516</v>
-      </c>
-      <c r="I12" s="49"/>
-      <c r="J12" s="20">
-        <f>SUM(J7:J11)</f>
-        <v>241260000</v>
-      </c>
-      <c r="K12" s="76"/>
-      <c r="L12" s="20">
-        <f>SUM(L7:L11)</f>
-        <v>120630000</v>
-      </c>
-      <c r="M12" s="49"/>
-      <c r="N12" s="49"/>
-      <c r="O12" s="20">
+      <c r="P11" s="41"/>
+      <c r="S11" s="76"/>
+    </row>
+    <row r="12" spans="1:21" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="98"/>
+      <c r="B12" s="105">
+        <v>44051</v>
+      </c>
+      <c r="C12" s="98"/>
+      <c r="D12" s="98" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="98" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="98"/>
+      <c r="G12" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" s="55">
+        <v>12</v>
+      </c>
+      <c r="I12" s="25">
+        <v>455000</v>
+      </c>
+      <c r="J12" s="56">
+        <f t="shared" ref="J12:J13" si="1">H12*I12</f>
+        <v>5460000</v>
+      </c>
+      <c r="K12" s="57">
+        <v>0.5</v>
+      </c>
+      <c r="L12" s="56">
+        <f t="shared" ref="L12:L13" si="2">J12*(1-K12)</f>
+        <v>2730000</v>
+      </c>
+      <c r="M12" s="58"/>
+      <c r="N12" s="58"/>
+      <c r="O12" s="59">
         <f t="shared" si="0"/>
-        <v>120630000</v>
-      </c>
-      <c r="P12" s="48"/>
-    </row>
-    <row r="13" spans="1:19" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="82"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="80"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-    </row>
-    <row r="14" spans="1:19" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>2730000</v>
+      </c>
+      <c r="P12" s="22"/>
+      <c r="S12" s="76"/>
+    </row>
+    <row r="13" spans="1:21" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="119"/>
+      <c r="B13" s="120"/>
+      <c r="C13" s="119"/>
+      <c r="D13" s="119"/>
+      <c r="E13" s="119"/>
+      <c r="F13" s="119"/>
+      <c r="G13" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="121">
+        <v>12</v>
+      </c>
+      <c r="I13" s="33">
+        <v>455000</v>
+      </c>
+      <c r="J13" s="122">
+        <f t="shared" si="1"/>
+        <v>5460000</v>
+      </c>
+      <c r="K13" s="123">
+        <v>0.5</v>
+      </c>
+      <c r="L13" s="122">
+        <f t="shared" si="2"/>
+        <v>2730000</v>
+      </c>
+      <c r="M13" s="124"/>
+      <c r="N13" s="124"/>
+      <c r="O13" s="125">
+        <f t="shared" si="0"/>
+        <v>2730000</v>
+      </c>
+      <c r="P13" s="32"/>
+      <c r="S13" s="76"/>
+    </row>
+    <row r="14" spans="1:21" s="47" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="82" t="s">
+        <v>41</v>
+      </c>
       <c r="B14" s="82"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="80"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="S14" s="106"/>
-    </row>
-    <row r="15" spans="1:19" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="77" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="78" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="78"/>
-      <c r="E15" s="78"/>
-      <c r="F15" s="78"/>
-      <c r="G15" s="79"/>
-      <c r="H15" s="103">
-        <f>'hàng nhập'!J31</f>
-        <v>620810000</v>
-      </c>
-      <c r="I15" s="103"/>
+      <c r="C14" s="82"/>
+      <c r="D14" s="82"/>
+      <c r="E14" s="82"/>
+      <c r="F14" s="82"/>
+      <c r="G14" s="82"/>
+      <c r="H14" s="44">
+        <f>SUM(H7:H13)</f>
+        <v>540</v>
+      </c>
+      <c r="I14" s="45"/>
+      <c r="J14" s="20">
+        <f>SUM(J7:J13)</f>
+        <v>252180000</v>
+      </c>
+      <c r="K14" s="70"/>
+      <c r="L14" s="20">
+        <f>SUM(L7:L13)</f>
+        <v>126090000</v>
+      </c>
+      <c r="M14" s="45"/>
+      <c r="N14" s="45"/>
+      <c r="O14" s="20">
+        <f>L14</f>
+        <v>126090000</v>
+      </c>
+      <c r="P14" s="44"/>
+      <c r="S14" s="131"/>
+    </row>
+    <row r="15" spans="1:21" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="76"/>
+      <c r="I15" s="8"/>
       <c r="J15" s="8"/>
-      <c r="K15" s="80"/>
+      <c r="K15" s="74"/>
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
       <c r="O15" s="8"/>
-    </row>
-    <row r="16" spans="1:19" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="82"/>
-      <c r="C16" s="83" t="s">
-        <v>46</v>
-      </c>
-      <c r="G16" s="81"/>
-      <c r="H16" s="103">
-        <f>J12</f>
-        <v>241260000</v>
-      </c>
-      <c r="I16" s="103"/>
+      <c r="S15" s="76"/>
+    </row>
+    <row r="16" spans="1:21" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="76"/>
+      <c r="I16" s="8"/>
       <c r="J16" s="8"/>
-      <c r="K16" s="80"/>
+      <c r="K16" s="74"/>
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
       <c r="N16" s="8"/>
       <c r="O16" s="8"/>
-    </row>
-    <row r="17" spans="2:15" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B17" s="82"/>
-      <c r="C17" s="104" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" s="104"/>
-      <c r="E17" s="104"/>
-      <c r="G17" s="84"/>
-      <c r="H17" s="105">
-        <f>(H15-H16)*0.5</f>
-        <v>189775000</v>
-      </c>
-      <c r="I17" s="105"/>
+      <c r="S16" s="76"/>
+    </row>
+    <row r="17" spans="2:20" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B17" s="71" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="72"/>
+      <c r="E17" s="72"/>
+      <c r="F17" s="72"/>
+      <c r="G17" s="73"/>
+      <c r="H17" s="96">
+        <f>'hàng nhập'!J40</f>
+        <v>1322930000</v>
+      </c>
+      <c r="I17" s="96"/>
       <c r="J17" s="8"/>
-      <c r="K17" s="80"/>
+      <c r="K17" s="74"/>
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
       <c r="O17" s="8"/>
-    </row>
-    <row r="18" spans="2:15" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="82"/>
-      <c r="I18" s="8"/>
+      <c r="S17" s="136" t="s">
+        <v>50</v>
+      </c>
+      <c r="T17" s="136"/>
+    </row>
+    <row r="18" spans="2:20" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B18" s="76"/>
+      <c r="C18" s="77" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="75"/>
+      <c r="H18" s="96">
+        <f>J14</f>
+        <v>252180000</v>
+      </c>
+      <c r="I18" s="96"/>
       <c r="J18" s="8"/>
-      <c r="K18" s="80"/>
+      <c r="K18" s="74"/>
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
       <c r="N18" s="8"/>
       <c r="O18" s="8"/>
+      <c r="S18" s="134">
+        <v>43659</v>
+      </c>
+      <c r="T18" s="135">
+        <v>150000000</v>
+      </c>
+    </row>
+    <row r="19" spans="2:20" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B19" s="76"/>
+      <c r="C19" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H19" s="126">
+        <f>H17-H18</f>
+        <v>1070750000</v>
+      </c>
+      <c r="I19" s="126"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="74"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="S19" s="134">
+        <v>43675</v>
+      </c>
+      <c r="T19" s="135">
+        <v>67000000</v>
+      </c>
+    </row>
+    <row r="20" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C20" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H20" s="128">
+        <f>H19*(1-50%)</f>
+        <v>535375000</v>
+      </c>
+      <c r="I20" s="127"/>
+      <c r="S20" s="134">
+        <v>44046</v>
+      </c>
+      <c r="T20" s="135">
+        <v>50000000</v>
+      </c>
+    </row>
+    <row r="21" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C21" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H21" s="133">
+        <f>T18+T19+T20+T21</f>
+        <v>367000000</v>
+      </c>
+      <c r="I21" s="133"/>
+      <c r="S21" s="134">
+        <v>44053</v>
+      </c>
+      <c r="T21" s="135">
+        <v>100000000</v>
+      </c>
+    </row>
+    <row r="22" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C22" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="137"/>
+      <c r="E22" s="137"/>
+      <c r="F22" s="137"/>
+      <c r="G22" s="137"/>
+      <c r="H22" s="138">
+        <f>H20-H21</f>
+        <v>168375000</v>
+      </c>
+      <c r="I22" s="139"/>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C23" s="137"/>
+      <c r="D23" s="137"/>
+      <c r="E23" s="137"/>
+      <c r="F23" s="137"/>
+      <c r="G23" s="137"/>
+      <c r="H23" s="137"/>
+      <c r="I23" s="137"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="A12:G12"/>
-    <mergeCell ref="H15:I15"/>
+  <mergeCells count="29">
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="S17:T17"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
     <mergeCell ref="A3:P3"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:B6"/>
@@ -2602,6 +3263,20 @@
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="G5:K5"/>
     <mergeCell ref="P5:P6"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="E7:E11"/>
+    <mergeCell ref="F7:F11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
   </mergeCells>
   <pageMargins left="0.2" right="0.2" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2612,7 +3287,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K27" sqref="K27:K28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>